<commit_message>
training for nn and lr started
</commit_message>
<xml_diff>
--- a/data/raw/heloc_data_dictionary-2.xlsx
+++ b/data/raw/heloc_data_dictionary-2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sriranjinilatha/Library/Application Support/Box/Box Edit/Documents/242398523088/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevencarlson/Desktop/Insight/explainableAI/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAC87C7-AA27-2B42-9478-5D04EE7344E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="920" windowWidth="24960" windowHeight="13720" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="640" yWindow="920" windowWidth="24960" windowHeight="13720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data Dictionary'!$A$1:$D$25</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -321,8 +322,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -456,6 +457,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -723,22 +727,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="43.5" style="7" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="57">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -752,7 +756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="32">
       <c r="A2" s="4" t="s">
         <v>58</v>
       </c>
@@ -764,7 +768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -786,7 +790,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
@@ -800,7 +804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -814,7 +818,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -828,7 +832,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="4" t="s">
         <v>48</v>
       </c>
@@ -842,7 +846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
@@ -856,7 +860,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" s="4" t="s">
         <v>50</v>
       </c>
@@ -870,7 +874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -884,7 +888,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -898,7 +902,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -912,7 +916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -926,7 +930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
@@ -940,7 +944,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
@@ -954,7 +958,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -968,7 +972,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -982,7 +986,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
         <v>53</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="4" t="s">
         <v>54</v>
       </c>
@@ -1010,7 +1014,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
@@ -1024,7 +1028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
@@ -1038,7 +1042,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
         <v>55</v>
       </c>
@@ -1052,7 +1056,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
@@ -1066,7 +1070,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
         <v>57</v>
       </c>
@@ -1080,7 +1084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
         <v>29</v>
       </c>
@@ -1094,42 +1098,42 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D25"/>
+  <autoFilter ref="A1:D25" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="12">
         <v>0</v>
       </c>
@@ -1137,7 +1141,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -1145,7 +1149,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="12">
         <v>2</v>
       </c>
@@ -1153,7 +1157,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="12">
         <v>3</v>
       </c>
@@ -1161,7 +1165,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="12">
         <v>4</v>
       </c>
@@ -1169,7 +1173,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="12" t="s">
         <v>71</v>
       </c>
@@ -1177,7 +1181,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="12">
         <v>7</v>
       </c>
@@ -1185,7 +1189,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="12" t="s">
         <v>75</v>
       </c>
@@ -1193,20 +1197,20 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="13"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="12">
         <v>1</v>
       </c>
@@ -1214,7 +1218,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="12">
         <v>2</v>
       </c>
@@ -1222,7 +1226,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="12">
         <v>3</v>
       </c>
@@ -1230,7 +1234,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="12">
         <v>4</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="12">
         <v>5</v>
       </c>
@@ -1246,7 +1250,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="12">
         <v>6</v>
       </c>
@@ -1254,7 +1258,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="12">
         <v>7</v>
       </c>
@@ -1262,7 +1266,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" s="12">
         <v>8</v>
       </c>
@@ -1270,7 +1274,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" s="12">
         <v>9</v>
       </c>
@@ -1284,26 +1288,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Fixed some bugs on nn and lr shap explain
</commit_message>
<xml_diff>
--- a/data/raw/heloc_data_dictionary-2.xlsx
+++ b/data/raw/heloc_data_dictionary-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevencarlson/Desktop/Insight/explainableAI/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAC87C7-AA27-2B42-9478-5D04EE7344E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7531BD5-549E-C34D-90C6-4E361DC49E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="920" windowWidth="24960" windowHeight="13720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="920" windowWidth="24960" windowHeight="13720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -730,19 +730,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112.83203125" customWidth="1"/>
     <col min="3" max="3" width="43.5" style="7" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="57">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="40">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -756,7 +756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32">
+    <row r="2" spans="1:12" ht="34">
       <c r="A2" s="4" t="s">
         <v>58</v>
       </c>
@@ -1115,7 +1115,7 @@
   <dimension ref="A2:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1291,7 +1291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>

</xml_diff>